<commit_message>
Cause List Update - Drug Overdose, and more
</commit_message>
<xml_diff>
--- a/myCCB/myInfo/Age Group Standard and US Standard 2000 Population.xlsx
+++ b/myCCB/myInfo/Age Group Standard and US Standard 2000 Population.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CCB\CCB Project\0.CCB\myCBD\myInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ACF694-BE95-4C30-94D6-35889086BD2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11656627-2E0E-4F04-954B-CB657ECD93CF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>https://www.cdc.gov/nchs/data/statnt/statnt20.pdf</t>
   </si>
@@ -94,6 +92,12 @@
   </si>
   <si>
     <t>65 - 999</t>
+  </si>
+  <si>
+    <t>Klein RJ, Schoenborn CA. Age adjustment using the 2000 projected U.S. population. Healthy People Statistical Notes, no. 20. Hyattsville, Maryland: National Center for Health Statistics. January 2001.</t>
+  </si>
+  <si>
+    <t>Table 2, Distribution #1, with under 1 year and 1-4 years combined</t>
   </si>
 </sst>
 </file>
@@ -488,7 +492,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,6 +656,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -659,7 +664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -745,11 +750,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -791,6 +794,16 @@
       <c r="B8">
         <f>SUM(B6:B7)</f>
         <v>18987</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -856,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>